<commit_message>
add opra and visa, update nbis and meta
</commit_message>
<xml_diff>
--- a/ACMR ACMS Stake.xlsx
+++ b/ACMR ACMS Stake.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerem\OneDrive\Masaüstü\Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EF595A7-CAB6-4ECE-8946-EA2C0B3D1ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D441FC6-8A93-4697-922F-883BD23D7F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12528" yWindow="696" windowWidth="27216" windowHeight="16008" xr2:uid="{849C67D8-495B-4707-99CA-8FAD1337D627}"/>
+    <workbookView xWindow="22944" yWindow="0" windowWidth="33432" windowHeight="16536" xr2:uid="{849C67D8-495B-4707-99CA-8FAD1337D627}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -342,10 +342,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -368,7 +367,7 @@
     <xf numFmtId="8" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -709,7 +708,7 @@
   <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -718,14 +717,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="15" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
@@ -733,99 +732,98 @@
       <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="16">
-        <v>3461</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="15">
+        <f>D5*D7</f>
+        <v>3763.04</v>
+      </c>
+      <c r="E3" s="2">
         <v>13611</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="17">
-        <v>3832</v>
-      </c>
-      <c r="E4" s="14">
+      <c r="C4" s="5"/>
+      <c r="D4" s="16">
+        <f>D5*D8</f>
+        <v>4165.5599999999995</v>
+      </c>
+      <c r="E4" s="13">
         <v>13855</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="20">
-        <v>53.36</v>
-      </c>
-      <c r="E5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="19">
+        <v>58</v>
+      </c>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="16">
-        <f>E4*0.75</f>
-        <v>10391.25</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="D6" s="15">
+        <f>E4*0.745</f>
+        <v>10321.975</v>
+      </c>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="16">
+      <c r="D7" s="15">
         <v>64.88</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="2:5" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="19">
+      <c r="C8" s="11"/>
+      <c r="D8" s="18">
         <v>71.819999999999993</v>
       </c>
-      <c r="E8" s="13"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="2:5" ht="14.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="18">
+      <c r="C9" s="5"/>
+      <c r="D9" s="17">
         <f>D6/D7</f>
-        <v>160.16106658446364</v>
-      </c>
-      <c r="E9" s="7"/>
+        <v>159.09332614056723</v>
+      </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="18">
+      <c r="C10" s="22"/>
+      <c r="D10" s="17">
         <f>D6/D8</f>
-        <v>144.68462823725983</v>
-      </c>
-      <c r="E10" s="23"/>
+        <v>143.72006404901143</v>
+      </c>
+      <c r="E10" s="22"/>
     </row>
     <row r="11" spans="2:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="24">
-        <f>D10/D5</f>
-        <v>2.7114810389291573</v>
-      </c>
-      <c r="E11" s="23"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="23">
+        <f>D10/D5-1</f>
+        <v>1.4779321387760591</v>
+      </c>
+      <c r="E11" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>